<commit_message>
--Changes in Code Upto Order Confirmation
</commit_message>
<xml_diff>
--- a/src/test/resources/com/travelex/nam/inputdatasheet/NAMDatasheet.xlsx
+++ b/src/test/resources/com/travelex/nam/inputdatasheet/NAMDatasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="18195" windowHeight="7050"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="18195" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="83">
   <si>
     <t>Scenario</t>
   </si>
@@ -192,9 +192,6 @@
     <t>PartnerID</t>
   </si>
   <si>
-    <t>CustomerType2</t>
-  </si>
-  <si>
     <t>ConfigQuoteAndViewBtn</t>
   </si>
   <si>
@@ -262,13 +259,43 @@
   </si>
   <si>
     <t>ConfigPrinterFriendlyBtn</t>
+  </si>
+  <si>
+    <t>CustomerRadioBtn</t>
+  </si>
+  <si>
+    <t>USD959CCC5</t>
+  </si>
+  <si>
+    <r>
+      <t>Pa$$word</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="56"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>AutoSaleOrder006</t>
+  </si>
+  <si>
+    <t>USD959CD10</t>
+  </si>
+  <si>
+    <t>USD959CD43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +354,18 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="56"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -365,7 +404,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -392,6 +431,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,7 +1155,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AK6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AK7" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <tableColumns count="37">
     <tableColumn id="1" name="AutomationID" dataDxfId="36"/>
     <tableColumn id="2" name="Scenario" dataDxfId="35"/>
@@ -1132,7 +1179,7 @@
     <tableColumn id="9" name="ConfigAddToOrder" dataDxfId="17"/>
     <tableColumn id="25" name="ConfigDeleteBtn" dataDxfId="16"/>
     <tableColumn id="24" name="ConfigConfirmBtn" dataDxfId="15"/>
-    <tableColumn id="18" name="CustomerType2" dataDxfId="14"/>
+    <tableColumn id="18" name="CustomerRadioBtn" dataDxfId="14"/>
     <tableColumn id="27" name="FirstName" dataDxfId="13"/>
     <tableColumn id="29" name="LastName" dataDxfId="12"/>
     <tableColumn id="28" name="GLAccNumber" dataDxfId="11"/>
@@ -1439,47 +1486,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK6"/>
+  <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4:AK6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="1" customWidth="1"/>
-    <col min="20" max="22" width="16.5703125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="27" width="12.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="12.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="19.140625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="19.28515625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="21.42578125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="18.28515625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="20.42578125" style="1" customWidth="1"/>
-    <col min="36" max="36" width="18.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="21.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="1" width="18.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
+    <col min="20" max="22" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="24" max="27" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="21.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="1" width="18.140625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="38" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -1526,7 +1573,7 @@
         <v>10</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>11</v>
@@ -1535,58 +1582,58 @@
         <v>12</v>
       </c>
       <c r="R1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AD1" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="AE1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="AJ1" s="4" t="s">
         <v>17</v>
@@ -1624,7 +1671,7 @@
         <v>52</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
@@ -1666,25 +1713,25 @@
         <v>16</v>
       </c>
       <c r="X2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>52</v>
@@ -1728,7 +1775,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>52</v>
@@ -1815,7 +1862,7 @@
         <v>52</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="AK3" s="10" t="s">
         <v>21</v>
@@ -1850,7 +1897,7 @@
         <v>52</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>14</v>
@@ -1963,7 +2010,7 @@
         <v>33</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>14</v>
@@ -2076,7 +2123,7 @@
         <v>38</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>14</v>
@@ -2158,16 +2205,130 @@
       </c>
       <c r="AK6" s="10" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="V7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK7" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
--Added Columns in Excel Sheet And Changes in Pages
</commit_message>
<xml_diff>
--- a/src/test/resources/com/travelex/nam/inputdatasheet/NAMDatasheet.xlsx
+++ b/src/test/resources/com/travelex/nam/inputdatasheet/NAMDatasheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="86">
   <si>
     <t>Scenario</t>
   </si>
@@ -264,30 +264,28 @@
     <t>CustomerRadioBtn</t>
   </si>
   <si>
-    <t>USD959CCC5</t>
-  </si>
-  <si>
-    <r>
-      <t>Pa$$word</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="56"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <t>AutoSaleOrder006</t>
-  </si>
-  <si>
-    <t>USD959CD10</t>
-  </si>
-  <si>
-    <t>USD959CD43</t>
+    <t>AutomationID_TC008</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>CANADA -- CAD</t>
+  </si>
+  <si>
+    <t>AttentionName</t>
+  </si>
+  <si>
+    <t>ConfigAlert</t>
+  </si>
+  <si>
+    <t>USD959CF95</t>
+  </si>
+  <si>
+    <t>USD959D064</t>
+  </si>
+  <si>
+    <t>USD959D06A</t>
   </si>
 </sst>
 </file>
@@ -295,7 +293,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,12 +353,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="56"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -404,7 +396,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -432,8 +424,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -445,7 +436,7 @@
     <cellStyle name="Normal 10" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="41">
     <dxf>
       <font>
         <b val="0"/>
@@ -566,6 +557,42 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -1155,36 +1182,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AK7" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <tableColumns count="37">
-    <tableColumn id="1" name="AutomationID" dataDxfId="36"/>
-    <tableColumn id="2" name="Scenario" dataDxfId="35"/>
-    <tableColumn id="3" name="LoginID" dataDxfId="34"/>
-    <tableColumn id="4" name="Password" dataDxfId="33"/>
-    <tableColumn id="21" name="PartnerID" dataDxfId="32"/>
-    <tableColumn id="7" name="CreateOrderType" dataDxfId="31"/>
-    <tableColumn id="8" name="ConfigOrderLink" dataDxfId="30"/>
-    <tableColumn id="10" name="BranchName" dataDxfId="29"/>
-    <tableColumn id="11" name="BranchLocation" dataDxfId="28"/>
-    <tableColumn id="12" name="ConfigConfirmCheckBox" dataDxfId="27"/>
-    <tableColumn id="13" name="TransactionType" dataDxfId="26"/>
-    <tableColumn id="5" name="CustomerType" dataDxfId="25"/>
-    <tableColumn id="14" name="ProductType" dataDxfId="24"/>
-    <tableColumn id="15" name="Currency" dataDxfId="23"/>
-    <tableColumn id="6" name="ConfigQuoteAndViewBtn" dataDxfId="22"/>
-    <tableColumn id="16" name="DomesticAmount" dataDxfId="21"/>
-    <tableColumn id="17" name="ForeignAmount" dataDxfId="20"/>
-    <tableColumn id="23" name="ConfigShowCurrency" dataDxfId="19"/>
-    <tableColumn id="22" name="ConfigClearFields" dataDxfId="18"/>
-    <tableColumn id="9" name="ConfigAddToOrder" dataDxfId="17"/>
-    <tableColumn id="25" name="ConfigDeleteBtn" dataDxfId="16"/>
-    <tableColumn id="24" name="ConfigConfirmBtn" dataDxfId="15"/>
-    <tableColumn id="18" name="CustomerRadioBtn" dataDxfId="14"/>
-    <tableColumn id="27" name="FirstName" dataDxfId="13"/>
-    <tableColumn id="29" name="LastName" dataDxfId="12"/>
-    <tableColumn id="28" name="GLAccNumber" dataDxfId="11"/>
-    <tableColumn id="30" name="BankID" dataDxfId="10"/>
-    <tableColumn id="31" name="SecurityID" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AM8" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:AM8">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="AutomationID_TC008"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="39">
+    <tableColumn id="1" name="AutomationID" dataDxfId="38"/>
+    <tableColumn id="2" name="Scenario" dataDxfId="37"/>
+    <tableColumn id="3" name="LoginID" dataDxfId="36"/>
+    <tableColumn id="4" name="Password" dataDxfId="35"/>
+    <tableColumn id="21" name="PartnerID" dataDxfId="34"/>
+    <tableColumn id="7" name="CreateOrderType" dataDxfId="33"/>
+    <tableColumn id="8" name="ConfigOrderLink" dataDxfId="32"/>
+    <tableColumn id="10" name="BranchName" dataDxfId="31"/>
+    <tableColumn id="11" name="BranchLocation" dataDxfId="30"/>
+    <tableColumn id="12" name="ConfigConfirmCheckBox" dataDxfId="29"/>
+    <tableColumn id="13" name="TransactionType" dataDxfId="28"/>
+    <tableColumn id="5" name="CustomerType" dataDxfId="27"/>
+    <tableColumn id="14" name="ProductType" dataDxfId="26"/>
+    <tableColumn id="15" name="Currency" dataDxfId="25"/>
+    <tableColumn id="6" name="ConfigQuoteAndViewBtn" dataDxfId="24"/>
+    <tableColumn id="16" name="DomesticAmount" dataDxfId="23"/>
+    <tableColumn id="17" name="ForeignAmount" dataDxfId="22"/>
+    <tableColumn id="23" name="ConfigShowCurrency" dataDxfId="21"/>
+    <tableColumn id="22" name="ConfigClearFields" dataDxfId="20"/>
+    <tableColumn id="9" name="ConfigAddToOrder" dataDxfId="19"/>
+    <tableColumn id="25" name="ConfigDeleteBtn" dataDxfId="18"/>
+    <tableColumn id="39" name="ConfigAlert" dataDxfId="17"/>
+    <tableColumn id="24" name="ConfigConfirmBtn" dataDxfId="16"/>
+    <tableColumn id="18" name="CustomerRadioBtn" dataDxfId="15"/>
+    <tableColumn id="27" name="FirstName" dataDxfId="14"/>
+    <tableColumn id="29" name="LastName" dataDxfId="13"/>
+    <tableColumn id="28" name="GLAccNumber" dataDxfId="12"/>
+    <tableColumn id="30" name="BankID" dataDxfId="11"/>
+    <tableColumn id="31" name="SecurityID" dataDxfId="10"/>
+    <tableColumn id="26" name="AttentionName" dataDxfId="9"/>
     <tableColumn id="33" name="BranchContact" dataDxfId="8"/>
     <tableColumn id="32" name="PhoneNumber" dataDxfId="7"/>
     <tableColumn id="36" name="ConfigChangeOrderBtn" dataDxfId="6"/>
@@ -1486,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1507,29 +1543,32 @@
     <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
     <col min="12" max="12" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
     <col min="15" max="15" customWidth="true" style="1" width="21.85546875" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
     <col min="18" max="18" customWidth="true" style="1" width="18.140625" collapsed="true"/>
     <col min="19" max="19" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
-    <col min="20" max="22" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="24" max="27" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="1" width="13.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" style="1" width="21.42578125" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="1" width="18.140625" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="38" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="20" max="21" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="25" max="28" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="1" width="21.42578125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="1" width="18.140625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="40" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -1594,55 +1633,61 @@
         <v>58</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1686,10 +1731,10 @@
         <v>18</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>19</v>
@@ -1706,39 +1751,35 @@
       <c r="U2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="W2" s="2" t="s">
+      <c r="V2" s="6"/>
+      <c r="W2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AB2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AC2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="AG2" s="1" t="s">
         <v>52</v>
       </c>
@@ -1751,11 +1792,17 @@
       <c r="AJ2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -1799,10 +1846,10 @@
         <v>18</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>19</v>
@@ -1819,15 +1866,13 @@
       <c r="U3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="W3" s="2" t="s">
+      <c r="V3" s="6"/>
+      <c r="W3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="Y3" s="2" t="s">
         <v>52</v>
       </c>
@@ -1843,13 +1888,11 @@
       <c r="AC3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF3" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AG3" s="1" t="s">
@@ -1862,13 +1905,19 @@
         <v>52</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK3" s="10" t="s">
-        <v>21</v>
+        <v>52</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM3" s="10" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1912,10 +1961,10 @@
         <v>30</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>31</v>
@@ -1932,15 +1981,13 @@
       <c r="U4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="2" t="s">
+      <c r="V4" s="6"/>
+      <c r="W4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X4" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="Y4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1956,13 +2003,11 @@
       <c r="AC4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AG4" s="1" t="s">
@@ -1977,11 +2022,17 @@
       <c r="AJ4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AK4" s="10" t="s">
+      <c r="AK4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -2025,10 +2076,10 @@
         <v>34</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>31</v>
@@ -2045,15 +2096,13 @@
       <c r="U5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="W5" s="2" t="s">
+      <c r="V5" s="6"/>
+      <c r="W5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="Y5" s="2" t="s">
         <v>52</v>
       </c>
@@ -2069,13 +2118,11 @@
       <c r="AC5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF5" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AG5" s="1" t="s">
@@ -2090,11 +2137,17 @@
       <c r="AJ5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AK5" s="10" t="s">
+      <c r="AK5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -2138,10 +2191,10 @@
         <v>39</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>31</v>
@@ -2158,15 +2211,13 @@
       <c r="U6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="W6" s="2" t="s">
+      <c r="V6" s="6"/>
+      <c r="W6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="X6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X6" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="Y6" s="2" t="s">
         <v>52</v>
       </c>
@@ -2182,13 +2233,11 @@
       <c r="AC6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AG6" s="1" t="s">
@@ -2203,24 +2252,30 @@
       <c r="AJ6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AK6" s="10" t="s">
+      <c r="AK6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>80</v>
+    <row r="7" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -2229,65 +2284,65 @@
       <c r="G7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="15" t="s">
+      <c r="H7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="10" t="s">
         <v>21</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="10" t="s">
+      <c r="L7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="10" t="s">
-        <v>18</v>
+      <c r="N7" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="T7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="U7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="V7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="W7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="X7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA7" s="10" t="s">
-        <v>52</v>
+      <c r="Y7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="AB7" s="10" t="s">
         <v>52</v>
@@ -2295,30 +2350,77 @@
       <c r="AC7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="AD7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ7" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK7" s="10" t="s">
+      <c r="AD7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI7" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="AJ7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM7" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>